<commit_message>
Add amount to drop table
</commit_message>
<xml_diff>
--- a/pack_world_game/design/Packs Items Tables.xlsx
+++ b/pack_world_game/design/Packs Items Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Archive\Game Development\Active\pack_world\pack_world_game\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3CFCB6-A61E-4BCB-A0B9-8FDC97E1BD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465D1001-9184-4C3C-AB81-FF3333846971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18165" yWindow="0" windowWidth="41070" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,27 +316,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -420,7 +400,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{333EBB11-1697-4271-B03A-E6B773563CFE}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{66779ED5-FBDC-43B6-B577-67F38636A1F1}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{80EF7A8F-4364-48E9-88BC-D9BE908A8E81}" name="%Chance" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{80EF7A8F-4364-48E9-88BC-D9BE908A8E81}" name="%Chance" dataDxfId="7" dataCellStyle="Percent">
       <calculatedColumnFormula>Table137891516[[#This Row],[Rate]]/SUM(Table137891516[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -434,7 +414,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{28E027C3-6619-4F6B-B9B5-4E991BEE7169}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{83798236-E790-4DCB-9325-19CBD2933987}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{80AE0A84-EBAE-467D-B0FF-B1661CD6F9CA}" name="%Chance" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{80AE0A84-EBAE-467D-B0FF-B1661CD6F9CA}" name="%Chance" dataDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1378918[[#This Row],[Rate]]/SUM(Table1378918[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -448,7 +428,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5710BAA2-303B-4130-B397-9E88F263AC1A}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{749EB946-237E-4C13-8450-9CB46D681F3D}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{29E82DC4-7FBA-46F8-A388-8832C45E81A7}" name="%Chance" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{29E82DC4-7FBA-46F8-A388-8832C45E81A7}" name="%Chance" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>Table137891819[[#This Row],[Rate]]/SUM(Table137891819[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -465,7 +445,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DFFD549D-06AC-4FEB-9CAE-81D867FAF7DA}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{5A314CBA-65C8-411D-9F89-C9E413B3C28A}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{D8F779D7-C1D3-4D6E-AE28-F4F37BF0FD4C}" name="%Chance" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{D8F779D7-C1D3-4D6E-AE28-F4F37BF0FD4C}" name="%Chance" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>Table137891520[[#This Row],[Rate]]/SUM(Table137891520[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -480,7 +460,7 @@
     <tableColumn id="1" xr3:uid="{BE923A95-75C9-4062-BE0B-A80844A43C74}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{8A2B068D-BA52-49A9-8B60-7C7AB68DE7AA}" name="Rate"/>
     <tableColumn id="4" xr3:uid="{96CED9DA-94ED-4108-8E34-6799C464E382}" name="Count"/>
-    <tableColumn id="3" xr3:uid="{B90E081D-90F4-47E6-B8F8-1845ADE3AC33}" name="%Chance" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{B90E081D-90F4-47E6-B8F8-1845ADE3AC33}" name="%Chance" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>Table13789181924[[#This Row],[Rate]]/SUM(Table13789181924[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -497,7 +477,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{381B99D4-DAE9-4E7B-B588-5D9988B19F22}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{D8C82624-656A-47EE-8246-49712DEB46B7}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{8A8DD7D9-1F12-4887-B5AA-12E962C2FD48}" name="%Chance" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{8A8DD7D9-1F12-4887-B5AA-12E962C2FD48}" name="%Chance" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1378915202[[#This Row],[Rate]]/SUM(Table1378915202[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -558,7 +538,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5FD88E56-EE50-4E96-AF7E-14BF06E4B5D5}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{45FE54DB-459E-467E-AEFD-A964A6E0ACBE}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{F15086BD-3ABF-42E8-AD67-1A721BE8BDB3}" name="%Chance" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{F15086BD-3ABF-42E8-AD67-1A721BE8BDB3}" name="%Chance" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>Table13789[[#This Row],[Rate]]/SUM(Table13789[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -572,7 +552,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B45D3A7A-5A1F-44F3-AEE5-F5F07020D270}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{8D0A6B32-E6FD-4FEB-BD6B-C5D482407A4D}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{C0196799-3FEE-40C1-A925-239F70EFBC90}" name="%Chance" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{C0196799-3FEE-40C1-A925-239F70EFBC90}" name="%Chance" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1378913[[#This Row],[Rate]]/SUM(Table1378913[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -587,7 +567,7 @@
     <tableColumn id="1" xr3:uid="{22D67FFD-FBB4-459B-A50A-FD89B7CA47EA}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{ABA1E863-6768-496A-992C-D3ACAA40AD3E}" name="Rate"/>
     <tableColumn id="6" xr3:uid="{21B42FB6-D1C6-45EA-99F9-B424D331BD57}" name="Count"/>
-    <tableColumn id="3" xr3:uid="{5F1A8B4E-B55C-46A2-AA78-2705E90B792F}" name="%Chance" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{5F1A8B4E-B55C-46A2-AA78-2705E90B792F}" name="%Chance" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>Table137891314[[#This Row],[Rate]]/SUM(Table137891314[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -604,7 +584,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{36F17566-CFEC-4201-BC32-CDFBEE168785}" name="ItemID"/>
     <tableColumn id="2" xr3:uid="{7FAF1644-E0BB-494D-A054-1BEBE28A02F9}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{5EBDFC1E-8AA4-45D3-B7A3-F1E8D0317C06}" name="%Chance" dataDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{5EBDFC1E-8AA4-45D3-B7A3-F1E8D0317C06}" name="%Chance" dataDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1378915[[#This Row],[Rate]]/SUM(Table1378915[Rate])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1224,7 +1204,7 @@
   <dimension ref="B4:X56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="AA39" sqref="AA39"/>
+      <selection activeCell="S50" sqref="S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
baby and dragon egg
</commit_message>
<xml_diff>
--- a/pack_world_game/design/Packs Items Tables.xlsx
+++ b/pack_world_game/design/Packs Items Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Archive\Game Development\Active\pack_world\pack_world_game\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44969E6F-DF73-42AA-AC8A-959DDC5BDDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F5AE6C-2ED8-4AEA-BA2D-3FA50E43069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18165" yWindow="0" windowWidth="41070" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="80">
   <si>
     <t>ItemID</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>Boulder</t>
+  </si>
+  <si>
+    <t>SmallGold</t>
   </si>
 </sst>
 </file>
@@ -1394,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB88C1E5-D251-4818-A177-3044F90F9570}">
   <dimension ref="B4:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,17 +1753,17 @@
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="F33">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G33">
         <v>20</v>
       </c>
       <c r="H33" s="4">
         <f>Table13789181924[[#This Row],[Rate]]/SUM(Table13789181924[Rate])</f>
-        <v>0.49875311720698251</v>
+        <v>0.62344139650872821</v>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
@@ -1768,14 +1771,14 @@
         <v>45</v>
       </c>
       <c r="F34">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34" s="4">
         <f>Table13789181924[[#This Row],[Rate]]/SUM(Table13789181924[Rate])</f>
-        <v>0.49875311720698251</v>
+        <v>0.37406483790523687</v>
       </c>
     </row>
     <row r="36" spans="5:8" ht="26.25" x14ac:dyDescent="0.4">
@@ -2074,7 +2077,7 @@
     </row>
     <row r="62" spans="5:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E62" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>

</xml_diff>

<commit_message>
grid layout for bank
</commit_message>
<xml_diff>
--- a/pack_world_game/design/Packs Items Tables.xlsx
+++ b/pack_world_game/design/Packs Items Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Archive\Game Development\Active\pack_world\pack_world_game\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C03F140-7F1C-4801-A7BE-5DBB76C99693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE24C42-A8DC-40AC-A097-43E89681C05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18165" yWindow="0" windowWidth="41070" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -990,7 +990,7 @@
   <dimension ref="D4:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add mud baby item
</commit_message>
<xml_diff>
--- a/pack_world_game/design/Packs Items Tables.xlsx
+++ b/pack_world_game/design/Packs Items Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Archive\Game Development\Active\pack_world\pack_world_game\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3FB153-9423-40D6-B123-5B72D243FFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45545700-590C-451D-A57B-88296409F180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18165" yWindow="0" windowWidth="41070" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="103">
   <si>
     <t>ItemID</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>TileTallGrass</t>
+  </si>
+  <si>
+    <t>MudBaby</t>
   </si>
 </sst>
 </file>
@@ -1659,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB88C1E5-D251-4818-A177-3044F90F9570}">
   <dimension ref="B2:X88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="S57" sqref="S57"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="T84" sqref="T84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,7 +2459,7 @@
       </c>
       <c r="N72" s="4">
         <f>Table13789131478[[#This Row],[Rate]]/SUM(Table13789131478[Rate])</f>
-        <v>0.49751243781094523</v>
+        <v>0.6211180124223602</v>
       </c>
     </row>
     <row r="73" spans="11:14" x14ac:dyDescent="0.25">
@@ -2471,7 +2474,7 @@
       </c>
       <c r="N73" s="4">
         <f>Table13789131478[[#This Row],[Rate]]/SUM(Table13789131478[Rate])</f>
-        <v>0.19900497512437809</v>
+        <v>0.24844720496894407</v>
       </c>
     </row>
     <row r="74" spans="11:14" x14ac:dyDescent="0.25">
@@ -2486,7 +2489,7 @@
       </c>
       <c r="N74" s="4">
         <f>Table13789131478[[#This Row],[Rate]]/SUM(Table13789131478[Rate])</f>
-        <v>4.9751243781094523E-2</v>
+        <v>6.2111801242236017E-2</v>
       </c>
     </row>
     <row r="75" spans="11:14" x14ac:dyDescent="0.25">
@@ -2501,22 +2504,22 @@
       </c>
       <c r="N75" s="4">
         <f>Table13789131478[[#This Row],[Rate]]/SUM(Table13789131478[Rate])</f>
-        <v>4.9751243781094526E-3</v>
+        <v>6.2111801242236021E-3</v>
       </c>
     </row>
     <row r="76" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K76" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="L76">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M76">
         <v>1</v>
       </c>
       <c r="N76" s="4">
         <f>Table13789131478[[#This Row],[Rate]]/SUM(Table13789131478[Rate])</f>
-        <v>0.24875621890547261</v>
+        <v>6.2111801242236017E-2</v>
       </c>
     </row>
     <row r="77" spans="11:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
support global drop mods
</commit_message>
<xml_diff>
--- a/pack_world_game/design/Packs Items Tables.xlsx
+++ b/pack_world_game/design/Packs Items Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Archive\Game Development\Active\pack_world\pack_world_game\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFC9655-230B-4322-A0E7-9FCC20734221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E2C03-4E89-4E47-A1B4-8489F986037C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18165" yWindow="0" windowWidth="41070" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2197,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB88C1E5-D251-4818-A177-3044F90F9570}">
   <dimension ref="B2:X110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="R93" sqref="R93"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>